<commit_message>
update tables based on new mutations model
</commit_message>
<xml_diff>
--- a/docs/resources/column_description.xlsx
+++ b/docs/resources/column_description.xlsx
@@ -368,9 +368,6 @@
     <t>the allele with minimal MHC I binding affinity of 9mer neoepitope candidate</t>
   </si>
   <si>
-    <t>the allele with minimal 9mer WT epitope  MHC I binding affinity</t>
-  </si>
-  <si>
     <t xml:space="preserve">Number of neoepitope candidates with MHC I binding affinity &lt; 50 nM per neoantigen canidate </t>
   </si>
   <si>
@@ -440,15 +437,6 @@
     <t>WT epitope with minimal MHC I binding rank score that corresponds to the general (8-11mers) best neoepitope candidate based on MHC I binding rank score</t>
   </si>
   <si>
-    <t>minimal MHC I binding rank score of 9mer WT epitope sequence that corresponds to the best 9mer neoepitope candidate based on MHC I binding rank score</t>
-  </si>
-  <si>
-    <t>9mer WT epitope with minimal MHC I binding rank score that corresponds to the best 9mer neoepitope candidate based on MHC I binding rank score</t>
-  </si>
-  <si>
-    <t>the allele with minimal  MHC I binding rank score related to 9mer WT epitope</t>
-  </si>
-  <si>
     <t>minimal MHC I binding affinity of 9mer WT epitope sequence that corresponds to the best 9mer neoepitope candidate based on MHC I binding affinity</t>
   </si>
   <si>
@@ -476,12 +464,6 @@
     <t>MHC II binding with netMHCIIpan</t>
   </si>
   <si>
-    <t>Harmonic mean of minimal MHC II binding rank scores to MHC II alleles</t>
-  </si>
-  <si>
-    <t>Harmonic mean of minimal MHC I binding rank scores to MHC I alleles</t>
-  </si>
-  <si>
     <t>Recognition Potential</t>
   </si>
   <si>
@@ -530,15 +512,6 @@
     <t>Difference of `Best_affinity_MHCI_score_WT` and `Best_affinity_MHCI_score`</t>
   </si>
   <si>
-    <t>Quotient of  `Best_affinity_MHCI_9mer_score_WT` and `Best_affinity_MHCI_9mer_score`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quotient of `Best_affinity_MHCI_score_WT` and `Best_affinity_MHCI_score` </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quotient of `Best_rank_MHCII_score_WT` and `Best_rank_MHCII_score` and </t>
-  </si>
-  <si>
     <t>Qutient of `Best_rank_MHCI_score_WT` and `Best_rank_MHCI_score`</t>
   </si>
   <si>
@@ -612,6 +585,33 @@
   </si>
   <si>
     <t>Feature group/ Paper</t>
+  </si>
+  <si>
+    <t>minimal MHC I binding rank score of 9mer WT epitope sequence that corresponds to the best 9mer neoepitope candidate based on MHC I binding rank score. The WT epitope should bind to the same MHC allele as the neoepitope candidate.</t>
+  </si>
+  <si>
+    <t>the allele with minimal  MHC I binding rank score related to 9mer WT epitope. The WT epitope should bind to the same MHC allele as the neoepitope candidate.The WT epitope should bind to the same MHC allele as the neoepitope candidate.</t>
+  </si>
+  <si>
+    <t>9mer WT epitope with minimal MHC I binding rank score that corresponds to the best 9mer neoepitope candidate based on MHC I binding rank score. The WT epitope should bind to the same MHC allele as the neoepitope candidate.</t>
+  </si>
+  <si>
+    <t>the allele with minimal 9mer WT epitope  MHC I binding affinity. The WT epitope should bind to the same MHC allele as the neoepitope candidate.</t>
+  </si>
+  <si>
+    <t>ratio of  `Best_affinity_MHCI_9mer_score_WT` and `Best_affinity_MHCI_9mer_score`</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratio of `Best_affinity_MHCI_score_WT` and `Best_affinity_MHCI_score` </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ratio of `Best_rank_MHCII_score_WT` and `Best_rank_MHCII_score` and </t>
+  </si>
+  <si>
+    <t>Harmonic mean of minimal MHC I binding rank scores of each MHC I alleles</t>
+  </si>
+  <si>
+    <t>Harmonic mean of minimal MHC II binding rank scores of each MHC II alleles</t>
   </si>
 </sst>
 </file>
@@ -965,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -984,7 +984,7 @@
         <v>87</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1135,7 +1135,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>107</v>
@@ -1204,7 +1204,7 @@
         <v>108</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30">
@@ -1212,7 +1212,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>109</v>
@@ -1223,7 +1223,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>109</v>
@@ -1245,7 +1245,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>109</v>
@@ -1256,7 +1256,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>109</v>
@@ -1278,7 +1278,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>109</v>
@@ -1289,7 +1289,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>109</v>
@@ -1311,7 +1311,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C31" s="6" t="s">
         <v>109</v>
@@ -1322,7 +1322,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C32" s="6" t="s">
         <v>109</v>
@@ -1344,7 +1344,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>109</v>
@@ -1355,7 +1355,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>109</v>
@@ -1366,7 +1366,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>109</v>
@@ -1377,7 +1377,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>109</v>
@@ -1388,7 +1388,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C38" s="6" t="s">
         <v>109</v>
@@ -1399,40 +1399,40 @@
         <v>37</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="45">
+    <row r="40" spans="1:3" ht="75">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>138</v>
+        <v>187</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="45">
+    <row r="41" spans="1:3" ht="60">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>139</v>
+        <v>189</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30">
+    <row r="42" spans="1:3" ht="75">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>140</v>
+        <v>188</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>109</v>
@@ -1443,7 +1443,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>109</v>
@@ -1454,18 +1454,18 @@
         <v>42</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="30">
+    <row r="45" spans="1:3" ht="45">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>114</v>
+        <v>190</v>
       </c>
       <c r="C45" s="6" t="s">
         <v>109</v>
@@ -1476,10 +1476,10 @@
         <v>44</v>
       </c>
       <c r="B46" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="30">
@@ -1487,7 +1487,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>151</v>
+        <v>194</v>
       </c>
       <c r="C47" s="6" t="s">
         <v>45</v>
@@ -1498,7 +1498,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C48" s="6" t="s">
         <v>109</v>
@@ -1506,13 +1506,13 @@
     </row>
     <row r="49" spans="1:3" ht="30">
       <c r="A49" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="30">
@@ -1520,10 +1520,10 @@
         <v>47</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="30">
@@ -1531,10 +1531,10 @@
         <v>48</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -1542,10 +1542,10 @@
         <v>49</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="30">
@@ -1553,10 +1553,10 @@
         <v>50</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="30">
@@ -1564,10 +1564,10 @@
         <v>51</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1575,10 +1575,10 @@
         <v>52</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="45">
@@ -1586,10 +1586,10 @@
         <v>53</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="45">
@@ -1597,10 +1597,10 @@
         <v>54</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1608,10 +1608,10 @@
         <v>55</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="45">
@@ -1619,10 +1619,10 @@
         <v>56</v>
       </c>
       <c r="B59" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C59" s="6" t="s">
         <v>145</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="45">
@@ -1630,10 +1630,10 @@
         <v>57</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1641,10 +1641,10 @@
         <v>58</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="30">
@@ -1652,7 +1652,7 @@
         <v>59</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>150</v>
+        <v>195</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>59</v>
@@ -1663,10 +1663,10 @@
         <v>60</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>168</v>
+        <v>191</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="30">
@@ -1674,21 +1674,21 @@
         <v>61</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>169</v>
+        <v>192</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="30">
       <c r="A65" s="4" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>170</v>
+        <v>193</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="45">
@@ -1696,10 +1696,10 @@
         <v>62</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="30">
@@ -1707,10 +1707,10 @@
         <v>63</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="30">
@@ -1718,10 +1718,10 @@
         <v>64</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1729,10 +1729,10 @@
         <v>65</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="30">
@@ -1740,10 +1740,10 @@
         <v>66</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1751,10 +1751,10 @@
         <v>67</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="30">
@@ -1762,10 +1762,10 @@
         <v>68</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1773,10 +1773,10 @@
         <v>69</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="30">
@@ -1784,10 +1784,10 @@
         <v>70</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="45">
@@ -1795,10 +1795,10 @@
         <v>71</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="45">
@@ -1806,10 +1806,10 @@
         <v>72</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="30">
@@ -1817,10 +1817,10 @@
         <v>73</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -1828,10 +1828,10 @@
         <v>74</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -1839,10 +1839,10 @@
         <v>75</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="45">
@@ -1850,10 +1850,10 @@
         <v>76</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="30">
@@ -1861,10 +1861,10 @@
         <v>77</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="82" spans="1:3">
@@ -1872,10 +1872,10 @@
         <v>78</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1883,10 +1883,10 @@
         <v>79</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="45">
@@ -1894,10 +1894,10 @@
         <v>80</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="30">
@@ -1905,10 +1905,10 @@
         <v>81</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1916,10 +1916,10 @@
         <v>82</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="30">
@@ -1927,10 +1927,10 @@
         <v>83</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="88" spans="1:3">
@@ -1938,10 +1938,10 @@
         <v>84</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="60">
@@ -1949,10 +1949,10 @@
         <v>85</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix some tests + update output data in the references
</commit_message>
<xml_diff>
--- a/docs/resources/column_description.xlsx
+++ b/docs/resources/column_description.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="214">
   <si>
     <t xml:space="preserve"> Column   Name                             </t>
   </si>
@@ -242,12 +242,6 @@
     <t xml:space="preserve"> ratio of   `Best_rank_MHCII_score_WT` and `Best_rank_MHCII_score` and                                                                                                                                                                            </t>
   </si>
   <si>
-    <t xml:space="preserve"> Pathogensimiliarity_MHCI_affinity_9mer    </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Recognition_Potential_MHCI_affinity_9mer  </t>
-  </si>
-  <si>
     <t xml:space="preserve"> product of   `Amplitude_MHCI_affinity_9mer` and `Pathogensimiliarity_MHCI_affinity_9mer`                                                                                                                                                         </t>
   </si>
   <si>
@@ -320,9 +314,6 @@
     <t xml:space="preserve"> neoag                           </t>
   </si>
   <si>
-    <t xml:space="preserve"> IEDB Immunogenicity score                                                                                                                                                                                                                        </t>
-  </si>
-  <si>
     <t xml:space="preserve"> IEDB Immunogenicity             </t>
   </si>
   <si>
@@ -623,13 +614,58 @@
     <t xml:space="preserve"> Dissimilarity_MHCI</t>
   </si>
   <si>
-    <t>hex_alignment_score</t>
-  </si>
-  <si>
-    <t>the alignment score by HEX</t>
-  </si>
-  <si>
     <t>HEX</t>
+  </si>
+  <si>
+    <t>Hex_alignment_score_MHCI</t>
+  </si>
+  <si>
+    <t>Hex_alignment_score_MHCII</t>
+  </si>
+  <si>
+    <t>the alignment score by HEX for ` Best_affinity_MHCII_epitope`</t>
+  </si>
+  <si>
+    <t>Dissimilarity_MHCII</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> score reflecting the   dissimilarity of `Best_affinity_MHCII_epitope` to the self-proteome                                                                                                                                                        </t>
+  </si>
+  <si>
+    <t>IEDB_Immunogenicity_MHCII</t>
+  </si>
+  <si>
+    <t>the alignment score by HEX for ` Best_affinity_MHCI_epitope `</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IEDB Immunogenicity score  for ` Best_affinity_MHCI_epitope `                                                                                                                                                                                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IEDB Immunogenicity score   for ` Best_affinity_MHCII_epitope`                                                                                                                                                                                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> score representing the   similarity of    `Best_affinity_MHCII_epitope` to pathogen sequences in IEDB   database                                                                                                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pathogensimiliarity_MHCI_9mer    </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Recognition_Potential_MHCI_9mer  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pathogensimiliarity_MHCII    </t>
+  </si>
+  <si>
+    <t>Selfsimilarity_MHCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> score representing the   similarity between `Best_rank_MHCI_score_epitope` and   `Best_affinity_MHCI_epitope_WT`   For conservered binder only                                                                                                                              </t>
+  </si>
+  <si>
+    <t>Selfsimilarity_MHCII</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> score representing the   similarity between `Best_affinity_MHCII_epitope` and    Best_affinity_MHCII_epitope_WT`                                                                                                                                 </t>
   </si>
 </sst>
 </file>
@@ -963,10 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B86" sqref="B86"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -991,7 +1027,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -1002,7 +1038,7 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -1013,7 +1049,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -1024,7 +1060,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1046,7 +1082,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
@@ -1057,7 +1093,7 @@
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1068,7 +1104,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -1090,7 +1126,7 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -1101,7 +1137,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -1112,7 +1148,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -1123,7 +1159,7 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C14" t="s">
         <v>20</v>
@@ -1134,7 +1170,7 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -1145,7 +1181,7 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -1153,10 +1189,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
@@ -1167,7 +1203,7 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C18" t="s">
         <v>20</v>
@@ -1178,7 +1214,7 @@
         <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C19" t="s">
         <v>20</v>
@@ -1189,7 +1225,7 @@
         <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
@@ -1200,7 +1236,7 @@
         <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
@@ -1211,7 +1247,7 @@
         <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C22" t="s">
         <v>20</v>
@@ -1222,7 +1258,7 @@
         <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C23" t="s">
         <v>20</v>
@@ -1233,7 +1269,7 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>
@@ -1244,7 +1280,7 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C25" t="s">
         <v>20</v>
@@ -1255,7 +1291,7 @@
         <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C26" t="s">
         <v>20</v>
@@ -1266,7 +1302,7 @@
         <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C27" t="s">
         <v>20</v>
@@ -1277,7 +1313,7 @@
         <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C28" t="s">
         <v>20</v>
@@ -1288,7 +1324,7 @@
         <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C29" t="s">
         <v>20</v>
@@ -1299,7 +1335,7 @@
         <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C30" t="s">
         <v>20</v>
@@ -1310,7 +1346,7 @@
         <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C31" t="s">
         <v>20</v>
@@ -1321,7 +1357,7 @@
         <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C32" t="s">
         <v>20</v>
@@ -1332,7 +1368,7 @@
         <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C33" t="s">
         <v>20</v>
@@ -1343,7 +1379,7 @@
         <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C34" t="s">
         <v>20</v>
@@ -1354,7 +1390,7 @@
         <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C35" t="s">
         <v>20</v>
@@ -1365,7 +1401,7 @@
         <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C36" t="s">
         <v>20</v>
@@ -1376,7 +1412,7 @@
         <v>45</v>
       </c>
       <c r="B37" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C37" t="s">
         <v>46</v>
@@ -1387,7 +1423,7 @@
         <v>47</v>
       </c>
       <c r="B38" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C38" t="s">
         <v>20</v>
@@ -1398,7 +1434,7 @@
         <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C39" t="s">
         <v>49</v>
@@ -1409,7 +1445,7 @@
         <v>50</v>
       </c>
       <c r="B40" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C40" t="s">
         <v>51</v>
@@ -1420,7 +1456,7 @@
         <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C41" t="s">
         <v>51</v>
@@ -1431,7 +1467,7 @@
         <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C42" t="s">
         <v>51</v>
@@ -1442,7 +1478,7 @@
         <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C43" t="s">
         <v>51</v>
@@ -1453,7 +1489,7 @@
         <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C44" t="s">
         <v>51</v>
@@ -1464,7 +1500,7 @@
         <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C45" t="s">
         <v>51</v>
@@ -1475,7 +1511,7 @@
         <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C46" t="s">
         <v>51</v>
@@ -1486,7 +1522,7 @@
         <v>58</v>
       </c>
       <c r="B47" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C47" t="s">
         <v>51</v>
@@ -1497,7 +1533,7 @@
         <v>59</v>
       </c>
       <c r="B48" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C48" t="s">
         <v>51</v>
@@ -1508,7 +1544,7 @@
         <v>60</v>
       </c>
       <c r="B49" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C49" t="s">
         <v>51</v>
@@ -1519,7 +1555,7 @@
         <v>61</v>
       </c>
       <c r="B50" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C50" t="s">
         <v>51</v>
@@ -1530,7 +1566,7 @@
         <v>62</v>
       </c>
       <c r="B51" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C51" t="s">
         <v>51</v>
@@ -1541,7 +1577,7 @@
         <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C52" t="s">
         <v>64</v>
@@ -1582,10 +1618,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>207</v>
       </c>
       <c r="B56" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C56" t="s">
         <v>67</v>
@@ -1593,10 +1629,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>209</v>
       </c>
       <c r="B57" t="s">
-        <v>74</v>
+        <v>206</v>
       </c>
       <c r="C57" t="s">
         <v>67</v>
@@ -1604,32 +1640,32 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="B58" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C58" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>190</v>
       </c>
       <c r="B59" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C59" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B60" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C60" t="s">
         <v>44</v>
@@ -1637,10 +1673,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C61" t="s">
         <v>44</v>
@@ -1648,21 +1684,21 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B62" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C62" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="1" t="s">
-        <v>122</v>
+      <c r="A63" t="s">
+        <v>81</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="C63" t="s">
         <v>44</v>
@@ -1670,10 +1706,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B64" t="s">
-        <v>125</v>
+        <v>43</v>
       </c>
       <c r="C64" t="s">
         <v>44</v>
@@ -1681,10 +1717,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B65" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C65" t="s">
         <v>44</v>
@@ -1692,10 +1728,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B66" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C66" t="s">
         <v>44</v>
@@ -1703,10 +1739,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B67" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C67" t="s">
         <v>44</v>
@@ -1714,255 +1750,321 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B68" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C68" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:3">
-      <c r="A69" t="s">
-        <v>194</v>
+      <c r="A69" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="B69" t="s">
-        <v>85</v>
+        <v>127</v>
       </c>
       <c r="C69" t="s">
-        <v>86</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>87</v>
+        <v>191</v>
       </c>
       <c r="B70" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C70" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B71" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C71" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B72" t="s">
-        <v>93</v>
+        <v>211</v>
       </c>
       <c r="C72" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" t="s">
-        <v>94</v>
+      <c r="A73" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="B73" t="s">
-        <v>195</v>
+        <v>89</v>
       </c>
       <c r="C73" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" t="s">
-        <v>95</v>
+      <c r="A74" s="1" t="s">
+        <v>212</v>
       </c>
       <c r="B74" t="s">
-        <v>96</v>
+        <v>213</v>
       </c>
       <c r="C74" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>197</v>
+        <v>90</v>
       </c>
       <c r="B75" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C75" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B76" t="s">
-        <v>101</v>
+        <v>192</v>
       </c>
       <c r="C76" t="s">
-        <v>102</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B77" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="C77" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>105</v>
+        <v>194</v>
       </c>
       <c r="B78" t="s">
-        <v>106</v>
+        <v>204</v>
       </c>
       <c r="C78" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" t="s">
-        <v>107</v>
+      <c r="A79" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="B79" t="s">
-        <v>108</v>
+        <v>205</v>
       </c>
       <c r="C79" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B80" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C80" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B81" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C81" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B82" t="s">
-        <v>196</v>
+        <v>103</v>
       </c>
       <c r="C82" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>198</v>
+        <v>104</v>
       </c>
       <c r="B83" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C83" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B84" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C84" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B85" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C85" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="B86" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="C86" t="s">
-        <v>133</v>
+        <v>108</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>136</v>
+        <v>195</v>
       </c>
       <c r="B87" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="C87" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" t="s">
-        <v>137</v>
+      <c r="A88" s="1" t="s">
+        <v>200</v>
       </c>
       <c r="B88" t="s">
-        <v>139</v>
+        <v>201</v>
       </c>
       <c r="C88" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
+        <v>114</v>
+      </c>
+      <c r="B89" t="s">
+        <v>115</v>
+      </c>
+      <c r="C89" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>117</v>
+      </c>
+      <c r="B90" t="s">
+        <v>118</v>
+      </c>
+      <c r="C90" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>132</v>
+      </c>
+      <c r="B91" t="s">
         <v>138</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C91" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>133</v>
+      </c>
+      <c r="B92" t="s">
+        <v>137</v>
+      </c>
+      <c r="C92" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
         <v>134</v>
       </c>
-      <c r="C89" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="2" t="s">
+      <c r="B93" t="s">
+        <v>136</v>
+      </c>
+      <c r="C93" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>135</v>
+      </c>
+      <c r="B94" t="s">
+        <v>131</v>
+      </c>
+      <c r="C94" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C95" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C90" t="s">
-        <v>201</v>
+      <c r="C96" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add fitness features for non 9mers
</commit_message>
<xml_diff>
--- a/docs/resources/column_description.xlsx
+++ b/docs/resources/column_description.xlsx
@@ -615,9 +615,6 @@
     <t xml:space="preserve"> Pathogensimiliarity_MHCII_bestAffinity</t>
   </si>
   <si>
-    <t>RecognitionPotential_bestAffinity9mer</t>
-  </si>
-  <si>
     <t xml:space="preserve"> ImprovedBinder_MHCI                      </t>
   </si>
   <si>
@@ -625,6 +622,9 @@
   </si>
   <si>
     <t>Vaxrank_bindingScore</t>
+  </si>
+  <si>
+    <t>RecognitionPotential_MHCI_bestAffinity9mer</t>
   </si>
 </sst>
 </file>
@@ -973,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1535,7 +1535,7 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="4" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="B51" t="s">
         <v>28</v>
@@ -1678,7 +1678,7 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B64" t="s">
         <v>37</v>
@@ -1876,7 +1876,7 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B82" t="s">
         <v>58</v>
@@ -1887,7 +1887,7 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B83" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
update col names in neoag table
</commit_message>
<xml_diff>
--- a/docs/resources/column_description.xlsx
+++ b/docs/resources/column_description.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="202">
   <si>
     <t xml:space="preserve"> Description                                                                                                                                                                                                                                      </t>
   </si>
@@ -99,63 +99,30 @@
     <t xml:space="preserve"> PHBR-II                         </t>
   </si>
   <si>
-    <t xml:space="preserve"> ratio of  `Best_affinity_MHCI_9mer_score_WT` and   `Best_affinity_MHCI_9mer_score`                                                                                                                                                               </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Recognition Potential           </t>
   </si>
   <si>
-    <t xml:space="preserve"> ratio of   `Best_affinity_MHCI_score_WT` and `Best_affinity_MHCI_score`                                                                                                                                                                          </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ratio of   `Best_rank_MHCII_score_WT` and `Best_rank_MHCII_score` and                                                                                                                                                                            </t>
-  </si>
-  <si>
     <t xml:space="preserve"> product of   `Amplitude_MHCI_affinity_9mer` and `Pathogensimiliarity_MHCI_affinity_9mer`                                                                                                                                                         </t>
   </si>
   <si>
-    <t xml:space="preserve"> difference of   `Best_affinity_MHCI_score_WT` and `Best_affinity_MHCI_score`                                                                                                                                                                     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> DAI                             </t>
   </si>
   <si>
-    <t xml:space="preserve"> `Best_affinity_MHCI_score` &lt;   50 nM                                                                                                                                                                                                             </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> `Best_affinity_MHCI_score` &lt;   5000 nM and `Amplitude_MHCI_affinity` &gt; 10                                                                                                                                                                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> `Best_rank_MHCII_score` &lt; 1                                                                                                                                                                                                                      </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> `Best_rank_MHCII_score` &lt; 4   and `Amplitude_MHCII_rank` &lt; 2                                                                                                                                                                                     </t>
-  </si>
-  <si>
     <t xml:space="preserve"> output score of T cell predictor   model                                                                                                                                                                                                         </t>
   </si>
   <si>
     <t xml:space="preserve"> Tcell predictor                 </t>
   </si>
   <si>
-    <t xml:space="preserve"> ratio of   `Best_rank_MHCI_score_WT` and `Best_rank_MHCI_score` &gt; 1.2                                                                                                                                                                           </t>
-  </si>
-  <si>
     <t xml:space="preserve"> self-similarity                 </t>
   </si>
   <si>
     <t xml:space="preserve"> Selfsimilarity_MHCI_conserved_binder      </t>
   </si>
   <si>
-    <t xml:space="preserve"> score representing the   similarity between `Best_rank_MHCI_score_epitope` and   `Best_affinity_MHCI_epitope_WT`                                                                                                                                 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Number_of_mismatches_MCHI                 </t>
   </si>
   <si>
-    <t xml:space="preserve"> number of amino acids that do no   match between `Best_rank_MHCI_score_epitope` and   `Best_rank_MHCI_score_epitope_WT`                                                                                                                          </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Priority_score                            </t>
   </si>
   <si>
@@ -180,9 +147,6 @@
     <t xml:space="preserve"> maximum MixMHCpred score over   all neoepitope canidates (8-11mers) and MHC I alleles                                                                                                                                                            </t>
   </si>
   <si>
-    <t xml:space="preserve"> rank that corresponds to   `MixMHCpred_best_score`                                                                                                                                                                                               </t>
-  </si>
-  <si>
     <t xml:space="preserve"> the allele with maximum   MixMHCpred score                                                                                                                                                                                                       </t>
   </si>
   <si>
@@ -195,9 +159,6 @@
     <t xml:space="preserve"> minimal MixMHC2pred score over   all neoepitope canidates (13-18mers) and MHC II alleles                                                                                                                                                         </t>
   </si>
   <si>
-    <t xml:space="preserve"> score reflecting the   dissimilarity of `Best_affinity_MHCI_epitope` to the self-proteome                                                                                                                                                        </t>
-  </si>
-  <si>
     <t xml:space="preserve"> dissimilarity                   </t>
   </si>
   <si>
@@ -213,12 +174,6 @@
     <t xml:space="preserve"> number of neoepitope candidates  with MHC I binding affinity &lt; 5000 nM per neoantigen canidate 10x better affinity in comparison to corresponding WT peptide                                                                                                                                                  </t>
   </si>
   <si>
-    <t>sum of `Generator_rate_CDN_MHCI` and `Generator_rate_ADN_MHCI`</t>
-  </si>
-  <si>
-    <t>sum of `Generator_rate_CDN_MHCII` and `Generator_rate_ADN_MHCII`</t>
-  </si>
-  <si>
     <t xml:space="preserve"> number of neoepitope candidates  with MHC II binding rank score &lt; 4 per neoantigen candidate 4x better rank in comparison to corresponding WT peptide                                                                                                                                                  </t>
   </si>
   <si>
@@ -270,18 +225,12 @@
     <t xml:space="preserve"> neoepitope candidate sequence with minimal MHC I binding rank score                                                                                                                                                                            </t>
   </si>
   <si>
-    <t xml:space="preserve"> the MHC I allele related to ` Best_rank_MHCI_score_epitope`                                                                                                                                                                  </t>
-  </si>
-  <si>
     <t xml:space="preserve"> minimal MHC I binding affinity  over all neoepitope candidates (8-11mers) and MHC I alleles                                                                                                                                                   </t>
   </si>
   <si>
     <t xml:space="preserve"> neoepitope candidate sequence with minimal MHC I binding affinity                                                                                                                                                                              </t>
   </si>
   <si>
-    <t xml:space="preserve"> the MHC I allele related to ` Best_affinity_MHCI_epitope`                                                                                                                                                                  </t>
-  </si>
-  <si>
     <t xml:space="preserve"> minimal MHC I binding rank score over all neoepitope candidates (9mers only) and MHC I alleles                                                                                                                                                  </t>
   </si>
   <si>
@@ -291,54 +240,15 @@
     <t xml:space="preserve"> minimal MHC I binding affinity over all neoepitope candidates (9mers) and MHC I alleles                                                                                                                                                          </t>
   </si>
   <si>
-    <t xml:space="preserve"> the MHC I allele related to ` Best_affinity_MHCI_9mer_epitope           `                                                                                                                                                                  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the MHC I allele related to ` Best_rank_MHCI_9mer_epitope`                                                                                                                                                                  </t>
-  </si>
-  <si>
     <t xml:space="preserve"> neoepitope candidate sequence (9mer) with minimal MHC I binding affinity                                                                                                                                                                    </t>
   </si>
   <si>
-    <t xml:space="preserve"> WT epitope that corresponds to ` Best_affinity_MHCI_epitope`</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MHC I binding affinity  of `Best_affinity_MHCI_epitope_WT`                                           </t>
-  </si>
-  <si>
-    <t>MHC I binding rank score of `Best_rank_MHCI_score_epitope_WT`</t>
-  </si>
-  <si>
-    <t>MHC I binding rank score of `Best_rank_MHCI_9mer_epitope_WT `</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> WT epitope that corresponds to `Best_rank_MHCI_9mer_epitope`</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> WT epitope that corresponds to `Best_rank_MHCI_score_epitope`</t>
-  </si>
-  <si>
     <t xml:space="preserve"> harmonic mean of minimal MHC I binding rank scores of all MHC I alleles of a patient                                                                                                                                                              </t>
   </si>
   <si>
-    <t>MHC I binding affinity of ` Best_affinity_MHCI_9mer_allele_WT `</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> WT epitope that corresponds to `Best_affinity_MHCI_9mer_epitope`</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> indicates position of the mutation in ` Best_affinity_MHCI_9mer_epitope`                                                                                                                                   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mutation in ` Best_affinity_MHCI_9mer_epitope` in an anchor position (i.e. position 2 or 9)                                                                                                                                                         </t>
-  </si>
-  <si>
     <t xml:space="preserve"> minimal MHC II binding rank score over all neoepitope candidates (15mers) and all MHC II alleles                                                                                                                                               </t>
   </si>
   <si>
-    <t xml:space="preserve"> the MHC II isoform related to ` Best_rank_MHCII_score_epitope`                                                                                                                                                                 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> neoepitope candidate sequence with minimal MHC II binding rank score                                                                                                                                                                   </t>
   </si>
   <si>
@@ -348,27 +258,9 @@
     <t xml:space="preserve"> minimal MHC II binding affinity  over all neoepitope candidates (15mers) and all MHC II alleles                                                                                                                                              </t>
   </si>
   <si>
-    <t xml:space="preserve"> the MHC II isoform related to ` Best_affinity_MHCII_epitope `                                                                                                                                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> WT epitope sequence (15mer) that corresponds to ` Best_rank_MHCII_score_epitope `</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> minimal MHC II binding rank of  `Best_rank_MHCII_score_epitope_WT  `</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> WT epitope sequence (15mer) that corresponds to `  Best_affinity_MHCII_epitope`</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> minimal MHC II binding rank of  `Best_affinity_MHCII_epitope_WT`</t>
-  </si>
-  <si>
     <t xml:space="preserve"> harmonic mean of minimal MHC II binding rank scores of all MHC II alleles of a patient                                                                                                                                                              </t>
   </si>
   <si>
-    <t xml:space="preserve"> score representing the   similarity of    `Best_affinity_MHCI_9mer_epitope` to pathogen sequences in IEDB   database                                                                                                                            </t>
-  </si>
-  <si>
     <t xml:space="preserve"> combinatorial score of several   features such as MHC binding, expression and VAF                                                                                                                                                                </t>
   </si>
   <si>
@@ -378,42 +270,18 @@
     <t>HEX</t>
   </si>
   <si>
-    <t>the alignment score by HEX for ` Best_affinity_MHCII_epitope`</t>
-  </si>
-  <si>
     <t>Dissimilarity_MHCII</t>
   </si>
   <si>
-    <t xml:space="preserve"> score reflecting the   dissimilarity of `Best_affinity_MHCII_epitope` to the self-proteome                                                                                                                                                        </t>
-  </si>
-  <si>
     <t>IEDB_Immunogenicity_MHCII</t>
   </si>
   <si>
-    <t>the alignment score by HEX for ` Best_affinity_MHCI_epitope `</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IEDB Immunogenicity score  for ` Best_affinity_MHCI_epitope `                                                                                                                                                                                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IEDB Immunogenicity score   for ` Best_affinity_MHCII_epitope`                                                                                                                                                                                                            </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> score representing the   similarity of    `Best_affinity_MHCII_epitope` to pathogen sequences in IEDB   database                                                                                                                            </t>
-  </si>
-  <si>
     <t>Selfsimilarity_MHCI</t>
   </si>
   <si>
-    <t xml:space="preserve"> score representing the   similarity between `Best_rank_MHCI_score_epitope` and   `Best_affinity_MHCI_epitope_WT`   For conservered binder only                                                                                                                              </t>
-  </si>
-  <si>
     <t>Selfsimilarity_MHCII</t>
   </si>
   <si>
-    <t xml:space="preserve"> score representing the   similarity between `Best_affinity_MHCII_epitope` and    Best_affinity_MHCII_epitope_WT`                                                                                                                                 </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Column  name                             </t>
   </si>
   <si>
@@ -625,6 +493,144 @@
   </si>
   <si>
     <t>RecognitionPotential_MHCI_bestAffinity9mer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the MHC I allele related to ` NetMHCpan_bestRank_peptide`                                                                                                                                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the MHC I allele related to ` NetMHCpan_bestAffinity_peptide`                                                                                                                                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the MHC I allele related to `NetMHCpan_bestRank9mer_peptide`                                                                                                                                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the MHC I allele related to ` NetMHCpan_bestAffinity9mer_peptide           `                                                                                                                                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MHC I binding affinity  of `NetMHCpan_bestAffinity_peptideWT`                                           </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WT epitope that corresponds to ` NetMHCpan_bestAffinity_peptide`</t>
+  </si>
+  <si>
+    <t>MHC I binding rank score of `NetMHCpan_bestRank_peptideWT`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WT epitope that corresponds to `NetMHCpan_bestRank_peptide`</t>
+  </si>
+  <si>
+    <t>MHC I binding rank score of `NetMHCpan_bestRank9mer_peptideWT `</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WT epitope that corresponds to `NetMHCpan_bestAffinity9mer_peptide`</t>
+  </si>
+  <si>
+    <t>NetMHCpan_bestAffinity9mer_peptideWT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MHC I binding rank score of  `NetMHCpan_bestAffinity9mer_peptideWT`</t>
+  </si>
+  <si>
+    <t>MHC I binding affinity of ` NetMHCpan_bestAffinity9mer_peptideWT `</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WT epitope that corresponds to `NetMHCpan_bestRank9mer_peptide`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> indicates position of the mutation in ` NetMHCpan_bestRank9mer_peptide`                                                                                                                                   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mutation in ` NetMHCpan_bestRank9mer_peptide` in an anchor position (i.e. position 2 or 9)                                                                                                                                                         </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the MHC II isoform related to `NetMHCIIpan_bestRank_peptide`                                                                                                                                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the MHC II isoform related to ` NetMHCIIpan_bestAffinity_peptide`                                                                                                                                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> minimal MHC II binding rank of  `NetMHCIIpan_bestRank_peptideWT`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WT epitope sequence (15mer) that corresponds to ` NetMHCIIpan_bestRank_peptide`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> minimal MHC II binding rank of  `NetMHCIIpan_bestAffinity_peptideWT`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> WT epitope sequence (15mer) that corresponds to `NetMHCIIpan_bestAffinity_peptide`</t>
+  </si>
+  <si>
+    <t>the alignment score by HEX for ` NetMHCIIpan_bestAffinity_peptide`</t>
+  </si>
+  <si>
+    <t>the alignment score by HEX for `NetMHCpan_bestAffinity_peptide`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> score reflecting the   dissimilarity of `NetMHCpan_bestAffinity_peptide` to the self-proteome                                                                                                                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> score reflecting the   dissimilarity of `NetMHCIIpan_bestAffinity_peptide` to the self-proteome                                                                                                                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rank that corresponds to   `MixMHCpred_bestScore_score`                                                                                                                                                                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IEDB Immunogenicity score  for ` NetMHCpan_bestAffinity_peptide`                                                                                                                                                                                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IEDB Immunogenicity score   for `NetMHCIIpan_bestAffinity_peptide`                                                                                                                                                                                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">`NetMHCpan_bestAffinity_peptide`&lt;   50 nM                                                                                                                                                                                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">`NetMHCpan_bestAffinity_peptide` &lt;   5000 nM and `Amplitude_MHCI_bestAffinity` &gt; 10                                                                                                                                                                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> `NetMHCIIpan_bestRank_rank` &lt; 1                                                                                                                                                                                                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> `Best_rank_MHCII_score` &lt; 4   and `Amplitude_MHCII_bestRank` &lt; 2                                                                                                                                                                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> score representing the   similarity of    `NetMHCpan_bestAffinity9mer_peptide` to pathogen sequences in IEDB   database                                                                                                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> score representing the   similarity of    `NetMHCIIpan_bestRank_peptide` to pathogen sequences in IEDB   database                                                                                                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> difference of   `NetMHCpan_bestAffinity_affinityWT` and `NetMHCpan_bestAffinity_affinity`                                                                                                                                                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ratio of   `NetMHCpan_bestAffinity_affinityWT` and `NetMHCpan_bestAffinity_affinity`                                                                                                                                                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ratio of  `NetMHCpan_bestAffinity9mer_affinity` and   `NetMHCpan_bestAffinity9mer_affinityWT`                                                                                                                                                               </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ratio of   `NetMHCIIpan_bestRank_rank` and `NetMHCIIpan_bestRank_rankWT`                                                                                                                                                                             </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ratio of   `NetMHCpan_MHCI_rank_bestRankWT` and `NetMHCpan_MHCI_rank_bestRank` &gt; 1.2                                                                                                                                                                           </t>
+  </si>
+  <si>
+    <t>sum of `GeneratorRate_CDN_MHCI` and `GeneratorRate_ADN_MHCI`</t>
+  </si>
+  <si>
+    <t>sum of `GeneratorRate_CDN_MHCII` and `GeneratorRate_ADN_MHCII`</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> score representing the   similarity between `NetMHCpan_bestRank_peptide` and   `NetMHCpan_bestRank_peptideWT`   For conservered binder only                                                                                                                              </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> score representing the   similarity between `NetMHCpan_bestRank_peptide` and   `NetMHCpan_bestRank_peptide`                                                                                                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> score representing the   similarity between `NetMHCIIpan_bestAffinity_peptide` and    `NetMHCIIpan_bestAffinity_peptide`                                                                                                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> number of amino acids that do no   match between `NetMHCpan_bestRank_peptide` and   `NetMHCpan_bestRank_peptideWT`                                                                                                          </t>
   </si>
 </sst>
 </file>
@@ -971,21 +977,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="50.140625" customWidth="1"/>
-    <col min="2" max="2" width="92" customWidth="1"/>
+    <col min="2" max="2" width="111.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -999,7 +1005,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -1010,7 +1016,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -1021,7 +1027,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1043,7 +1049,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -1054,7 +1060,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -1065,7 +1071,7 @@
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
@@ -1087,7 +1093,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -1098,7 +1104,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C11" t="s">
         <v>16</v>
@@ -1106,10 +1112,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="4" t="s">
-        <v>152</v>
+        <v>108</v>
       </c>
       <c r="B12" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -1117,10 +1123,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
-        <v>153</v>
+        <v>109</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
@@ -1128,10 +1134,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
-        <v>154</v>
+        <v>110</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>156</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -1139,10 +1145,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
-        <v>157</v>
+        <v>113</v>
       </c>
       <c r="B15" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
@@ -1150,10 +1156,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
-        <v>158</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
@@ -1161,10 +1167,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
-        <v>159</v>
+        <v>115</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>157</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -1172,10 +1178,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
-        <v>162</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -1183,10 +1189,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
       <c r="B19" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -1194,10 +1200,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
-        <v>164</v>
+        <v>120</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>158</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -1205,10 +1211,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
-        <v>167</v>
+        <v>123</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -1216,10 +1222,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="3" t="s">
-        <v>168</v>
+        <v>124</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>159</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -1227,10 +1233,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
-        <v>169</v>
+        <v>125</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -1238,10 +1244,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" t="s">
         <v>160</v>
-      </c>
-      <c r="B24" t="s">
-        <v>92</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
@@ -1249,10 +1255,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" t="s">
         <v>161</v>
-      </c>
-      <c r="B25" t="s">
-        <v>91</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
@@ -1260,10 +1266,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="3" t="s">
-        <v>155</v>
+        <v>111</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
@@ -1271,10 +1277,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="3" t="s">
-        <v>156</v>
+        <v>112</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>163</v>
       </c>
       <c r="C27" t="s">
         <v>17</v>
@@ -1282,10 +1288,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="3" t="s">
-        <v>165</v>
+        <v>121</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>164</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
@@ -1293,10 +1299,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="3" t="s">
-        <v>166</v>
+        <v>122</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>169</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
@@ -1304,10 +1310,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="3" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>168</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
@@ -1315,65 +1321,62 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="3" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="B31" t="s">
-        <v>99</v>
+        <v>167</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="4" t="s">
-        <v>172</v>
+      <c r="A32" s="3" t="s">
+        <v>166</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B33" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="3" t="s">
-        <v>177</v>
+        <v>132</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>170</v>
       </c>
       <c r="C34" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>171</v>
       </c>
       <c r="C35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="3" t="s">
-        <v>138</v>
+        <v>93</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="C36" t="s">
         <v>22</v>
@@ -1381,10 +1384,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="3" t="s">
-        <v>139</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="C37" t="s">
         <v>22</v>
@@ -1392,10 +1395,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="3" t="s">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="B38" t="s">
-        <v>106</v>
+        <v>172</v>
       </c>
       <c r="C38" t="s">
         <v>22</v>
@@ -1403,10 +1406,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="3" t="s">
-        <v>143</v>
+        <v>98</v>
       </c>
       <c r="B39" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="C39" t="s">
         <v>22</v>
@@ -1414,10 +1417,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="3" t="s">
-        <v>144</v>
+        <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
         <v>22</v>
@@ -1425,10 +1428,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="3" t="s">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="B41" t="s">
-        <v>109</v>
+        <v>173</v>
       </c>
       <c r="C41" t="s">
         <v>22</v>
@@ -1436,10 +1439,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="3" t="s">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>174</v>
       </c>
       <c r="C42" t="s">
         <v>22</v>
@@ -1447,10 +1450,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="3" t="s">
-        <v>145</v>
+        <v>97</v>
       </c>
       <c r="B43" t="s">
-        <v>111</v>
+        <v>175</v>
       </c>
       <c r="C43" t="s">
         <v>22</v>
@@ -1458,10 +1461,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="3" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="B44" t="s">
-        <v>110</v>
+        <v>176</v>
       </c>
       <c r="C44" t="s">
         <v>22</v>
@@ -1469,109 +1472,109 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="3" t="s">
-        <v>147</v>
+        <v>102</v>
       </c>
       <c r="B45" t="s">
-        <v>112</v>
+        <v>177</v>
       </c>
       <c r="C45" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="3" t="s">
-        <v>182</v>
+        <v>103</v>
       </c>
       <c r="B46" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="C46" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="3" t="s">
-        <v>183</v>
+        <v>138</v>
       </c>
       <c r="B47" t="s">
-        <v>26</v>
+        <v>193</v>
       </c>
       <c r="C47" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="3" t="s">
-        <v>184</v>
+        <v>139</v>
       </c>
       <c r="B48" t="s">
-        <v>27</v>
+        <v>192</v>
       </c>
       <c r="C48" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:3">
-      <c r="A49" t="s">
+      <c r="A49" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49" t="s">
         <v>194</v>
       </c>
-      <c r="B49" t="s">
-        <v>113</v>
-      </c>
       <c r="C49" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>195</v>
+        <v>150</v>
       </c>
       <c r="B50" t="s">
-        <v>124</v>
+        <v>189</v>
       </c>
       <c r="C50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>151</v>
+      </c>
+      <c r="B51" t="s">
+        <v>190</v>
+      </c>
+      <c r="C51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B52" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="B51" t="s">
-        <v>28</v>
-      </c>
-      <c r="C51" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" t="s">
-        <v>185</v>
-      </c>
-      <c r="B52" t="s">
-        <v>29</v>
-      </c>
       <c r="C52" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>188</v>
+        <v>141</v>
       </c>
       <c r="B53" t="s">
-        <v>31</v>
+        <v>191</v>
       </c>
       <c r="C53" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>186</v>
+        <v>144</v>
       </c>
       <c r="B54" t="s">
-        <v>32</v>
+        <v>185</v>
       </c>
       <c r="C54" t="s">
         <v>19</v>
@@ -1579,10 +1582,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>189</v>
+        <v>142</v>
       </c>
       <c r="B55" t="s">
-        <v>33</v>
+        <v>186</v>
       </c>
       <c r="C55" t="s">
         <v>19</v>
@@ -1590,21 +1593,21 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
+        <v>145</v>
+      </c>
+      <c r="B56" t="s">
         <v>187</v>
-      </c>
-      <c r="B56" t="s">
-        <v>34</v>
       </c>
       <c r="C56" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="57" spans="1:3">
-      <c r="A57" s="4" t="s">
-        <v>173</v>
+      <c r="A57" t="s">
+        <v>143</v>
       </c>
       <c r="B57" t="s">
-        <v>18</v>
+        <v>188</v>
       </c>
       <c r="C57" t="s">
         <v>19</v>
@@ -1612,10 +1615,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="4" t="s">
-        <v>174</v>
+        <v>129</v>
       </c>
       <c r="B58" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="C58" t="s">
         <v>19</v>
@@ -1623,10 +1626,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="4" t="s">
-        <v>175</v>
+        <v>130</v>
       </c>
       <c r="B59" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C59" t="s">
         <v>19</v>
@@ -1634,10 +1637,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="4" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B60" t="s">
-        <v>65</v>
+        <v>196</v>
       </c>
       <c r="C60" t="s">
         <v>19</v>
@@ -1645,10 +1648,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="4" t="s">
-        <v>150</v>
+        <v>105</v>
       </c>
       <c r="B61" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C61" t="s">
         <v>19</v>
@@ -1656,87 +1659,87 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="4" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C62" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" t="s">
-        <v>151</v>
+      <c r="A63" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="B63" t="s">
-        <v>35</v>
+        <v>197</v>
       </c>
       <c r="C63" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>196</v>
+        <v>107</v>
       </c>
       <c r="B64" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C64" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>39</v>
+        <v>152</v>
       </c>
       <c r="B65" t="s">
-        <v>126</v>
+        <v>195</v>
       </c>
       <c r="C65" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" s="1" t="s">
-        <v>125</v>
+      <c r="A66" t="s">
+        <v>30</v>
       </c>
       <c r="B66" t="s">
-        <v>40</v>
+        <v>198</v>
       </c>
       <c r="C66" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="1" t="s">
-        <v>127</v>
+        <v>83</v>
       </c>
       <c r="B67" t="s">
-        <v>128</v>
+        <v>199</v>
       </c>
       <c r="C67" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" t="s">
-        <v>41</v>
+      <c r="A68" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="B68" t="s">
-        <v>42</v>
+        <v>200</v>
       </c>
       <c r="C68" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B69" t="s">
-        <v>114</v>
+        <v>201</v>
       </c>
       <c r="C69" t="s">
         <v>16</v>
@@ -1744,222 +1747,233 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B70" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="C70" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>193</v>
+        <v>33</v>
       </c>
       <c r="B71" t="s">
-        <v>122</v>
+        <v>34</v>
       </c>
       <c r="C71" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="1" t="s">
-        <v>120</v>
+      <c r="A72" t="s">
+        <v>149</v>
       </c>
       <c r="B72" t="s">
-        <v>123</v>
+        <v>183</v>
       </c>
       <c r="C72" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="3" t="s">
-        <v>133</v>
+      <c r="A73" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="B73" t="s">
-        <v>48</v>
+        <v>184</v>
       </c>
       <c r="C73" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="3" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="B74" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C74" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="3" t="s">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="B75" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C75" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="3" t="s">
-        <v>136</v>
+        <v>91</v>
       </c>
       <c r="B76" t="s">
-        <v>52</v>
+        <v>182</v>
       </c>
       <c r="C76" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="3" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="B77" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C77" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="3" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="B78" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C78" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="3" t="s">
-        <v>132</v>
+        <v>87</v>
       </c>
       <c r="B79" t="s">
-        <v>115</v>
+        <v>43</v>
       </c>
       <c r="C79" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" t="s">
-        <v>190</v>
+      <c r="A80" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="B80" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="C80" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="1" t="s">
-        <v>118</v>
+      <c r="A81" t="s">
+        <v>146</v>
       </c>
       <c r="B81" t="s">
-        <v>119</v>
+        <v>180</v>
       </c>
       <c r="C81" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="3" t="s">
-        <v>198</v>
+      <c r="A82" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>58</v>
+        <v>181</v>
       </c>
       <c r="C82" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" t="s">
-        <v>197</v>
+      <c r="A83" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="B83" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C83" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" s="3" t="s">
-        <v>180</v>
+      <c r="A84" t="s">
+        <v>153</v>
       </c>
       <c r="B84" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="C84" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="3" t="s">
-        <v>181</v>
+        <v>136</v>
       </c>
       <c r="B85" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C85" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="3" t="s">
-        <v>179</v>
+        <v>137</v>
       </c>
       <c r="B86" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C86" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="3" t="s">
-        <v>178</v>
+        <v>135</v>
       </c>
       <c r="B87" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C87" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
     </row>
     <row r="88" spans="1:3">
-      <c r="A88" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>121</v>
+      <c r="A88" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B88" t="s">
+        <v>52</v>
       </c>
       <c r="C88" t="s">
-        <v>116</v>
+        <v>51</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="1" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>117</v>
+        <v>179</v>
       </c>
       <c r="C89" t="s">
-        <v>116</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C90" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added netMHCpan additional annotations and column descriptions
</commit_message>
<xml_diff>
--- a/docs/resources/column_description.xlsx
+++ b/docs/resources/column_description.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mz-zdv-s-nfs001.unimedizin-mainz.ext\projects$\SUMMIT\WP1.2\input\addanot_clone\input_v0.2.0\docs\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CM01_iVAC\neomouse_test\neofox\neofox_repo\docs\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21735" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="Neoantigen" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="223">
   <si>
     <t xml:space="preserve"> Description                                                                                                                                                                                                                                      </t>
   </si>
@@ -351,9 +351,6 @@
     <t xml:space="preserve"> Tcell_predictor</t>
   </si>
   <si>
-    <t>NetMHCpan_MHCI_rank_bestRank</t>
-  </si>
-  <si>
     <t>NetMHCpan_bestRank_peptide</t>
   </si>
   <si>
@@ -631,13 +628,79 @@
   </si>
   <si>
     <t xml:space="preserve"> number of amino acids that do no   match between `NetMHCpan_bestRank_peptide` and   `NetMHCpan_bestRank_peptideWT`                                                                                                          </t>
+  </si>
+  <si>
+    <t>NetMHCpan_bestRank_rank</t>
+  </si>
+  <si>
+    <t>NetMHCpan_bestRank_core</t>
+  </si>
+  <si>
+    <t>The minimal 9 amino acid binding core directly in contact with the MHC.</t>
+  </si>
+  <si>
+    <t>NetMHCpan_bestRank_Icore</t>
+  </si>
+  <si>
+    <t>Interaction core. This is the sequence of the binding core including eventual insertions of deletions.</t>
+  </si>
+  <si>
+    <t>NetMHCpan_bestRank_Gp</t>
+  </si>
+  <si>
+    <t>NetMHCpan_bestRank_Gl</t>
+  </si>
+  <si>
+    <t>Length of the deletion, if any, in the Icore compared to the core.</t>
+  </si>
+  <si>
+    <t>Position of the deletion (0 based), if any, in the Icore compared to the core.</t>
+  </si>
+  <si>
+    <t>NetMHCpan_bestAffinity_core</t>
+  </si>
+  <si>
+    <t>NetMHCpan_bestAffinity_Icore</t>
+  </si>
+  <si>
+    <t>NetMHCpan_bestAffinity_Gp</t>
+  </si>
+  <si>
+    <t>NetMHCpan_bestAffinity_Gl</t>
+  </si>
+  <si>
+    <t>NetMHCIIpan_bestRank_core</t>
+  </si>
+  <si>
+    <t>NetMHCIIpan_bestRank_Of</t>
+  </si>
+  <si>
+    <t>NetMHCIIpan_bestRank_coreRel</t>
+  </si>
+  <si>
+    <t>Binding core register (9mer)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starting position offset of the optimal binding core (starting from 0) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reliability of the binding core, expressed as the fraction of networks in the ensemble selecting the optimal core </t>
+  </si>
+  <si>
+    <t>NetMHCIIpan_bestAffinity_core</t>
+  </si>
+  <si>
+    <t>NetMHCIIpan_bestAffinity_Of</t>
+  </si>
+  <si>
+    <t>NetMHCIIpan_bestAffinity_coreRel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -666,6 +729,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -687,7 +757,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -697,6 +767,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -977,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1111,8 +1182,8 @@
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="4" t="s">
-        <v>108</v>
+      <c r="A12" s="3" t="s">
+        <v>201</v>
       </c>
       <c r="B12" t="s">
         <v>64</v>
@@ -1123,7 +1194,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
         <v>65</v>
@@ -1134,10 +1205,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
-        <v>110</v>
+        <v>202</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>203</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -1145,10 +1216,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
-        <v>113</v>
+        <v>204</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>205</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
@@ -1156,10 +1227,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
-        <v>114</v>
+        <v>206</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>209</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
@@ -1167,10 +1238,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
-        <v>115</v>
+        <v>207</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>208</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -1178,10 +1249,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>155</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -1189,10 +1260,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -1200,10 +1271,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B20" t="s">
-        <v>158</v>
+        <v>67</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -1211,10 +1282,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
-        <v>123</v>
+        <v>210</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>203</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -1222,10 +1293,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="3" t="s">
-        <v>124</v>
+        <v>211</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>205</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -1233,10 +1304,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
-        <v>125</v>
+        <v>212</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>209</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -1244,10 +1315,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
-        <v>116</v>
+        <v>213</v>
       </c>
       <c r="B24" t="s">
-        <v>160</v>
+        <v>208</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
@@ -1255,10 +1326,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B25" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
@@ -1266,10 +1337,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="3" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B26" t="s">
-        <v>162</v>
+        <v>68</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
@@ -1277,10 +1348,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="3" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B27" t="s">
-        <v>163</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
         <v>17</v>
@@ -1288,10 +1359,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B28" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
@@ -1302,7 +1373,7 @@
         <v>122</v>
       </c>
       <c r="B29" t="s">
-        <v>169</v>
+        <v>70</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
@@ -1310,10 +1381,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B30" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
@@ -1321,10 +1392,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B31" t="s">
-        <v>167</v>
+        <v>71</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
@@ -1332,29 +1403,32 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="3" t="s">
-        <v>166</v>
+        <v>115</v>
       </c>
       <c r="B32" t="s">
-        <v>165</v>
+        <v>159</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="4" t="s">
-        <v>128</v>
+      <c r="A33" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>160</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="3" t="s">
-        <v>132</v>
+        <v>110</v>
       </c>
       <c r="B34" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C34" t="s">
         <v>17</v>
@@ -1362,109 +1436,106 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="3" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="B35" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C35" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="3" t="s">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="B36" t="s">
-        <v>73</v>
+        <v>163</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="3" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>168</v>
       </c>
       <c r="C37" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="3" t="s">
-        <v>95</v>
+        <v>126</v>
       </c>
       <c r="B38" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C38" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="3" t="s">
-        <v>98</v>
+        <v>125</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>166</v>
       </c>
       <c r="C39" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="3" t="s">
-        <v>99</v>
+        <v>165</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
-      </c>
-      <c r="C40" t="s">
-        <v>22</v>
+        <v>164</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="3" t="s">
-        <v>100</v>
+      <c r="A41" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="B41" t="s">
-        <v>173</v>
+        <v>72</v>
       </c>
       <c r="C41" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="3" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="B42" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C42" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="3" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="B43" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B44" t="s">
-        <v>176</v>
+        <v>73</v>
       </c>
       <c r="C44" t="s">
         <v>22</v>
@@ -1472,208 +1543,208 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="3" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B45" t="s">
-        <v>177</v>
+        <v>74</v>
       </c>
       <c r="C45" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" ht="15.75">
       <c r="A46" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B46" t="s">
-        <v>77</v>
+        <v>214</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>217</v>
       </c>
       <c r="C46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="15.75">
       <c r="A47" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B47" t="s">
-        <v>193</v>
+        <v>215</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>218</v>
       </c>
       <c r="C47" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="15.75">
       <c r="A48" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B48" t="s">
-        <v>192</v>
+        <v>216</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>219</v>
       </c>
       <c r="C48" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="3" t="s">
-        <v>140</v>
+        <v>95</v>
       </c>
       <c r="B49" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="C49" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>150</v>
+      <c r="A50" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>189</v>
+        <v>76</v>
       </c>
       <c r="C50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15.75">
+      <c r="A52" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C52" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15.75">
+      <c r="A53" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="C53" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15.75">
+      <c r="A54" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C54" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B55" t="s">
+        <v>172</v>
+      </c>
+      <c r="C55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" t="s">
+        <v>173</v>
+      </c>
+      <c r="C56" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B57" t="s">
+        <v>174</v>
+      </c>
+      <c r="C57" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B58" t="s">
+        <v>175</v>
+      </c>
+      <c r="C58" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B59" t="s">
+        <v>176</v>
+      </c>
+      <c r="C59" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B60" t="s">
+        <v>77</v>
+      </c>
+      <c r="C60" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B61" t="s">
+        <v>192</v>
+      </c>
+      <c r="C61" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" t="s">
-        <v>151</v>
-      </c>
-      <c r="B51" t="s">
-        <v>190</v>
-      </c>
-      <c r="C51" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B52" t="s">
-        <v>25</v>
-      </c>
-      <c r="C52" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" t="s">
-        <v>141</v>
-      </c>
-      <c r="B53" t="s">
+    <row r="62" spans="1:3">
+      <c r="A62" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B62" t="s">
         <v>191</v>
-      </c>
-      <c r="C53" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" t="s">
-        <v>144</v>
-      </c>
-      <c r="B54" t="s">
-        <v>185</v>
-      </c>
-      <c r="C54" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>142</v>
-      </c>
-      <c r="B55" t="s">
-        <v>186</v>
-      </c>
-      <c r="C55" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" t="s">
-        <v>145</v>
-      </c>
-      <c r="B56" t="s">
-        <v>187</v>
-      </c>
-      <c r="C56" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
-        <v>143</v>
-      </c>
-      <c r="B57" t="s">
-        <v>188</v>
-      </c>
-      <c r="C57" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B58" t="s">
-        <v>18</v>
-      </c>
-      <c r="C58" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B59" t="s">
-        <v>48</v>
-      </c>
-      <c r="C59" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B60" t="s">
-        <v>196</v>
-      </c>
-      <c r="C60" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B61" t="s">
-        <v>50</v>
-      </c>
-      <c r="C61" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B62" t="s">
-        <v>49</v>
       </c>
       <c r="C62" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="63" spans="1:3">
-      <c r="A63" s="4" t="s">
-        <v>104</v>
+      <c r="A63" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="B63" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="C63" t="s">
         <v>19</v>
@@ -1681,298 +1752,452 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>107</v>
+        <v>149</v>
       </c>
       <c r="B64" t="s">
-        <v>27</v>
+        <v>188</v>
       </c>
       <c r="C64" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B65" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C65" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" spans="1:3">
-      <c r="A66" t="s">
-        <v>30</v>
+      <c r="A66" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="B66" t="s">
-        <v>198</v>
+        <v>25</v>
       </c>
       <c r="C66" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:3">
-      <c r="A67" s="1" t="s">
-        <v>83</v>
+      <c r="A67" t="s">
+        <v>140</v>
       </c>
       <c r="B67" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C67" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" s="1" t="s">
-        <v>84</v>
+      <c r="A68" t="s">
+        <v>143</v>
       </c>
       <c r="B68" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="C68" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>31</v>
+        <v>141</v>
       </c>
       <c r="B69" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="C69" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
+        <v>186</v>
       </c>
       <c r="C70" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>33</v>
+        <v>142</v>
       </c>
       <c r="B71" t="s">
-        <v>34</v>
+        <v>187</v>
       </c>
       <c r="C71" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" t="s">
-        <v>149</v>
+      <c r="A72" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="B72" t="s">
-        <v>183</v>
+        <v>18</v>
       </c>
       <c r="C72" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="1" t="s">
-        <v>82</v>
+      <c r="A73" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="B73" t="s">
-        <v>184</v>
+        <v>48</v>
       </c>
       <c r="C73" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="74" spans="1:3">
-      <c r="A74" s="3" t="s">
-        <v>89</v>
+      <c r="A74" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="B74" t="s">
-        <v>37</v>
+        <v>195</v>
       </c>
       <c r="C74" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="75" spans="1:3">
-      <c r="A75" s="3" t="s">
-        <v>90</v>
+      <c r="A75" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="B75" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C75" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="76" spans="1:3">
-      <c r="A76" s="3" t="s">
-        <v>91</v>
+      <c r="A76" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="B76" t="s">
-        <v>182</v>
+        <v>49</v>
       </c>
       <c r="C76" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="77" spans="1:3">
-      <c r="A77" s="3" t="s">
-        <v>92</v>
+      <c r="A77" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="B77" t="s">
-        <v>40</v>
+        <v>196</v>
       </c>
       <c r="C77" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" s="3" t="s">
-        <v>86</v>
+      <c r="A78" t="s">
+        <v>107</v>
       </c>
       <c r="B78" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C78" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" s="3" t="s">
-        <v>87</v>
+      <c r="A79" t="s">
+        <v>151</v>
       </c>
       <c r="B79" t="s">
-        <v>43</v>
+        <v>194</v>
       </c>
       <c r="C79" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="80" spans="1:3">
-      <c r="A80" s="3" t="s">
-        <v>88</v>
+      <c r="A80" t="s">
+        <v>30</v>
       </c>
       <c r="B80" t="s">
-        <v>79</v>
+        <v>197</v>
       </c>
       <c r="C80" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" t="s">
-        <v>146</v>
+      <c r="A81" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="B81" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="C81" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="C82" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" s="3" t="s">
-        <v>154</v>
+      <c r="A83" t="s">
+        <v>31</v>
       </c>
       <c r="B83" t="s">
-        <v>45</v>
+        <v>200</v>
       </c>
       <c r="C83" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>153</v>
+        <v>32</v>
       </c>
       <c r="B84" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="C84" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="A85" s="3" t="s">
-        <v>136</v>
+      <c r="A85" t="s">
+        <v>33</v>
       </c>
       <c r="B85" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="C85" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
     </row>
     <row r="86" spans="1:3">
-      <c r="A86" s="3" t="s">
-        <v>137</v>
+      <c r="A86" t="s">
+        <v>148</v>
       </c>
       <c r="B86" t="s">
-        <v>54</v>
+        <v>182</v>
       </c>
       <c r="C86" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="A87" s="3" t="s">
-        <v>135</v>
+      <c r="A87" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="B87" t="s">
-        <v>53</v>
+        <v>183</v>
       </c>
       <c r="C87" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88" t="s">
+        <v>37</v>
+      </c>
+      <c r="C88" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89" t="s">
+        <v>39</v>
+      </c>
+      <c r="C89" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90" t="s">
+        <v>181</v>
+      </c>
+      <c r="C90" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B91" t="s">
+        <v>40</v>
+      </c>
+      <c r="C91" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B92" t="s">
+        <v>41</v>
+      </c>
+      <c r="C92" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B93" t="s">
+        <v>43</v>
+      </c>
+      <c r="C93" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B94" t="s">
+        <v>79</v>
+      </c>
+      <c r="C94" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>145</v>
+      </c>
+      <c r="B95" t="s">
+        <v>179</v>
+      </c>
+      <c r="C95" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B96" t="s">
+        <v>180</v>
+      </c>
+      <c r="C96" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B97" t="s">
+        <v>45</v>
+      </c>
+      <c r="C97" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>152</v>
+      </c>
+      <c r="B98" t="s">
+        <v>47</v>
+      </c>
+      <c r="C98" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B99" t="s">
+        <v>55</v>
+      </c>
+      <c r="C99" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B100" t="s">
+        <v>54</v>
+      </c>
+      <c r="C100" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B101" t="s">
+        <v>53</v>
+      </c>
+      <c r="C101" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B102" t="s">
         <v>52</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C102" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="1" t="s">
+    <row r="103" spans="1:3">
+      <c r="A103" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C103" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C89" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C90" t="s">
+      <c r="B104" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C104" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added documentation for new columns. Method for NetMHCpan annotation extraction now static.
</commit_message>
<xml_diff>
--- a/docs/resources/column_description.xlsx
+++ b/docs/resources/column_description.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="226">
   <si>
     <t xml:space="preserve"> Description                                                                                                                                                                                                                                      </t>
   </si>
@@ -694,6 +694,15 @@
   </si>
   <si>
     <t>NetMHCIIpan_bestAffinity_coreRel</t>
+  </si>
+  <si>
+    <t>NetMHCpan_bestAffinity_Of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starting position offset of the core in the peptide (0 based) </t>
+  </si>
+  <si>
+    <t>NetMHCpan_bestRank_Of</t>
   </si>
 </sst>
 </file>
@@ -1048,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C104"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1227,10 +1236,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="B16" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
@@ -1238,10 +1247,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B17" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -1249,10 +1258,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
-        <v>109</v>
+        <v>207</v>
       </c>
       <c r="B18" t="s">
-        <v>155</v>
+        <v>208</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -1260,10 +1269,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>155</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -1271,10 +1280,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -1282,10 +1291,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
-        <v>210</v>
+        <v>113</v>
       </c>
       <c r="B21" t="s">
-        <v>203</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -1293,10 +1302,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B22" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -1304,10 +1313,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B23" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -1315,10 +1324,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="B24" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
@@ -1326,10 +1335,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="3" t="s">
-        <v>114</v>
+        <v>212</v>
       </c>
       <c r="B25" t="s">
-        <v>156</v>
+        <v>209</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
@@ -1337,10 +1346,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="3" t="s">
-        <v>117</v>
+        <v>213</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>208</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
@@ -1348,10 +1357,10 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>156</v>
       </c>
       <c r="C27" t="s">
         <v>17</v>
@@ -1359,10 +1368,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B28" t="s">
-        <v>157</v>
+        <v>68</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
@@ -1370,10 +1379,10 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
@@ -1381,10 +1390,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
@@ -1392,10 +1401,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
@@ -1403,10 +1412,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="3" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="B32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
@@ -1414,10 +1423,10 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="3" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="B33" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s">
         <v>17</v>
@@ -1425,10 +1434,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="3" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B34" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C34" t="s">
         <v>17</v>
@@ -1436,10 +1445,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C35" t="s">
         <v>17</v>
@@ -1447,10 +1456,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B36" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C36" t="s">
         <v>17</v>
@@ -1458,10 +1467,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="3" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B37" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="C37" t="s">
         <v>17</v>
@@ -1469,10 +1478,10 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="3" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B38" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C38" t="s">
         <v>17</v>
@@ -1480,10 +1489,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B39" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C39" t="s">
         <v>17</v>
@@ -1491,84 +1500,84 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="3" t="s">
-        <v>165</v>
+        <v>126</v>
       </c>
       <c r="B40" t="s">
-        <v>164</v>
+        <v>167</v>
+      </c>
+      <c r="C40" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="4" t="s">
-        <v>127</v>
+      <c r="A41" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>166</v>
       </c>
       <c r="C41" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="3" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="B42" t="s">
-        <v>169</v>
-      </c>
-      <c r="C42" t="s">
-        <v>17</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="3" t="s">
-        <v>132</v>
+      <c r="A43" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="B43" t="s">
-        <v>170</v>
+        <v>72</v>
       </c>
       <c r="C43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="3" t="s">
-        <v>93</v>
+        <v>131</v>
       </c>
       <c r="B44" t="s">
-        <v>73</v>
+        <v>169</v>
       </c>
       <c r="C44" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="3" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="B45" t="s">
-        <v>74</v>
+        <v>170</v>
       </c>
       <c r="C45" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>217</v>
+        <v>93</v>
+      </c>
+      <c r="B46" t="s">
+        <v>73</v>
       </c>
       <c r="C46" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15.75">
+    <row r="47" spans="1:3">
       <c r="A47" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>218</v>
+        <v>94</v>
+      </c>
+      <c r="B47" t="s">
+        <v>74</v>
       </c>
       <c r="C47" t="s">
         <v>22</v>
@@ -1576,32 +1585,32 @@
     </row>
     <row r="48" spans="1:3" ht="15.75">
       <c r="A48" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C48" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" ht="15.75">
       <c r="A49" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B49" t="s">
-        <v>171</v>
+        <v>215</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>218</v>
       </c>
       <c r="C49" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" ht="15.75">
       <c r="A50" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" t="s">
-        <v>76</v>
+        <v>216</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>219</v>
       </c>
       <c r="C50" t="s">
         <v>22</v>
@@ -1609,32 +1618,32 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B51" t="s">
-        <v>75</v>
+        <v>171</v>
       </c>
       <c r="C51" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="15.75">
+    <row r="52" spans="1:3">
       <c r="A52" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>217</v>
+        <v>98</v>
+      </c>
+      <c r="B52" t="s">
+        <v>76</v>
       </c>
       <c r="C52" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="15.75">
+    <row r="53" spans="1:3">
       <c r="A53" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="B53" s="5" t="s">
-        <v>218</v>
+        <v>99</v>
+      </c>
+      <c r="B53" t="s">
+        <v>75</v>
       </c>
       <c r="C53" t="s">
         <v>22</v>
@@ -1642,32 +1651,32 @@
     </row>
     <row r="54" spans="1:3" ht="15.75">
       <c r="A54" s="3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C54" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" ht="15.75">
       <c r="A55" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B55" t="s">
-        <v>172</v>
+        <v>221</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>218</v>
       </c>
       <c r="C55" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" ht="15.75">
       <c r="A56" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B56" t="s">
-        <v>173</v>
+        <v>222</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>219</v>
       </c>
       <c r="C56" t="s">
         <v>22</v>
@@ -1675,10 +1684,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="3" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B57" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C57" t="s">
         <v>22</v>
@@ -1686,10 +1695,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B58" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C58" t="s">
         <v>22</v>
@@ -1697,10 +1706,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B59" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C59" t="s">
         <v>22</v>
@@ -1708,76 +1717,76 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B60" t="s">
-        <v>77</v>
+        <v>175</v>
       </c>
       <c r="C60" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="3" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="B61" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="C61" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="3" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="B62" t="s">
-        <v>191</v>
+        <v>77</v>
       </c>
       <c r="C62" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B63" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B64" t="s">
+        <v>191</v>
+      </c>
+      <c r="C64" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B65" t="s">
         <v>193</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C65" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
         <v>149</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B66" t="s">
         <v>188</v>
-      </c>
-      <c r="C64" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
-        <v>150</v>
-      </c>
-      <c r="B65" t="s">
-        <v>189</v>
-      </c>
-      <c r="C65" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B66" t="s">
-        <v>25</v>
       </c>
       <c r="C66" t="s">
         <v>24</v>
@@ -1785,43 +1794,43 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="B67" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C67" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:3">
-      <c r="A68" t="s">
-        <v>143</v>
+      <c r="A68" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="B68" t="s">
-        <v>184</v>
+        <v>25</v>
       </c>
       <c r="C68" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B69" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="C69" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B70" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C70" t="s">
         <v>19</v>
@@ -1829,32 +1838,32 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B71" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C71" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="72" spans="1:3">
-      <c r="A72" s="4" t="s">
-        <v>128</v>
+      <c r="A72" t="s">
+        <v>144</v>
       </c>
       <c r="B72" t="s">
-        <v>18</v>
+        <v>186</v>
       </c>
       <c r="C72" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="73" spans="1:3">
-      <c r="A73" s="4" t="s">
-        <v>129</v>
+      <c r="A73" t="s">
+        <v>142</v>
       </c>
       <c r="B73" t="s">
-        <v>48</v>
+        <v>187</v>
       </c>
       <c r="C73" t="s">
         <v>19</v>
@@ -1862,10 +1871,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B74" t="s">
-        <v>195</v>
+        <v>18</v>
       </c>
       <c r="C74" t="s">
         <v>19</v>
@@ -1873,10 +1882,10 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="4" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="B75" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C75" t="s">
         <v>19</v>
@@ -1884,10 +1893,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="4" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="B76" t="s">
-        <v>49</v>
+        <v>195</v>
       </c>
       <c r="C76" t="s">
         <v>19</v>
@@ -1895,153 +1904,153 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B77" t="s">
-        <v>196</v>
+        <v>50</v>
       </c>
       <c r="C77" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:3">
-      <c r="A78" t="s">
-        <v>107</v>
+      <c r="A78" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C78" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="79" spans="1:3">
-      <c r="A79" t="s">
-        <v>151</v>
+      <c r="A79" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="B79" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C79" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>30</v>
+        <v>107</v>
       </c>
       <c r="B80" t="s">
-        <v>197</v>
+        <v>27</v>
       </c>
       <c r="C80" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="81" spans="1:3">
-      <c r="A81" s="1" t="s">
-        <v>83</v>
+      <c r="A81" t="s">
+        <v>151</v>
       </c>
       <c r="B81" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C81" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="82" spans="1:3">
-      <c r="A82" s="1" t="s">
-        <v>84</v>
+      <c r="A82" t="s">
+        <v>30</v>
       </c>
       <c r="B82" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C82" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="83" spans="1:3">
-      <c r="A83" t="s">
-        <v>31</v>
+      <c r="A83" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C83" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="84" spans="1:3">
-      <c r="A84" t="s">
-        <v>32</v>
+      <c r="A84" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>78</v>
+        <v>199</v>
       </c>
       <c r="C84" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B85" t="s">
-        <v>34</v>
+        <v>200</v>
       </c>
       <c r="C85" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
+        <v>32</v>
+      </c>
+      <c r="B86" t="s">
+        <v>78</v>
+      </c>
+      <c r="C86" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>33</v>
+      </c>
+      <c r="B87" t="s">
+        <v>34</v>
+      </c>
+      <c r="C87" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
         <v>148</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B88" t="s">
         <v>182</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C88" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="1" t="s">
+    <row r="89" spans="1:3">
+      <c r="A89" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B89" t="s">
         <v>183</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C89" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B88" t="s">
-        <v>37</v>
-      </c>
-      <c r="C88" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B89" t="s">
-        <v>39</v>
-      </c>
-      <c r="C89" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>181</v>
+        <v>37</v>
       </c>
       <c r="C90" t="s">
         <v>38</v>
@@ -2049,10 +2058,10 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C91" t="s">
         <v>38</v>
@@ -2060,109 +2069,109 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>41</v>
+        <v>181</v>
       </c>
       <c r="C92" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C93" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B94" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="C94" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="95" spans="1:3">
-      <c r="A95" t="s">
+      <c r="A95" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B95" t="s">
+        <v>43</v>
+      </c>
+      <c r="C95" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B96" t="s">
+        <v>79</v>
+      </c>
+      <c r="C96" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
         <v>145</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B97" t="s">
         <v>179</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C97" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
-      <c r="A96" s="1" t="s">
+    <row r="98" spans="1:3">
+      <c r="A98" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B98" t="s">
         <v>180</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C98" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B97" t="s">
-        <v>45</v>
-      </c>
-      <c r="C97" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" t="s">
-        <v>152</v>
-      </c>
-      <c r="B98" t="s">
-        <v>47</v>
-      </c>
-      <c r="C98" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="3" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="B99" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C99" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="100" spans="1:3">
-      <c r="A100" s="3" t="s">
-        <v>136</v>
+      <c r="A100" t="s">
+        <v>152</v>
       </c>
       <c r="B100" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C100" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B101" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C101" t="s">
         <v>51</v>
@@ -2170,34 +2179,56 @@
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B102" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C102" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="103" spans="1:3">
-      <c r="A103" s="1" t="s">
+      <c r="A103" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B103" t="s">
+        <v>53</v>
+      </c>
+      <c r="C103" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B104" t="s">
+        <v>52</v>
+      </c>
+      <c r="C104" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C105" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
-      <c r="A104" s="1" t="s">
+    <row r="106" spans="1:3">
+      <c r="A106" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B106" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C106" t="s">
         <v>80</v>
       </c>
     </row>

</xml_diff>